<commit_message>
Removing Bogus Comments and Adding Graphs
Removed a variety of worthless comments from the tests (inaccurate,
misspelled, etc.).  Added more analysis to the timing analysis file.
</commit_message>
<xml_diff>
--- a/manual_code/Context_Switching_UART/timer_analysis.xlsx
+++ b/manual_code/Context_Switching_UART/timer_analysis.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="out" sheetId="1" r:id="rId1"/>
+    <sheet name="Request Frequency" sheetId="3" r:id="rId1"/>
+    <sheet name="out" sheetId="1" r:id="rId2"/>
+    <sheet name="Line Graph" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Request</t>
   </si>
@@ -32,6 +34,24 @@
   </si>
   <si>
     <t>Mode:</t>
+  </si>
+  <si>
+    <t>Request Bin</t>
+  </si>
+  <si>
+    <t>Request Frequency</t>
+  </si>
+  <si>
+    <t>Send Bin</t>
+  </si>
+  <si>
+    <t>Send Frequency</t>
+  </si>
+  <si>
+    <t>Receive Bin</t>
+  </si>
+  <si>
+    <t>Receive Frequency</t>
   </si>
 </sst>
 </file>
@@ -569,6 +589,1289 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-CA"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Request</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Time Frequencies</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>out!$Q$2:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>out!$R$2:$R$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="121186560"/>
+        <c:axId val="121204736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="121186560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (microseconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121204736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="121204736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121186560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-CA"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Primitive Timing</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Request</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>out!$M$2:$M$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Send</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>out!$N$2:$N$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Receive</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>out!$O$2:$O$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="49719552"/>
+        <c:axId val="49733632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49719552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Trial</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49733632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49733632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (microseconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49719552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="85" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="74" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656996" cy="6298790"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8654815" cy="6291204"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -854,15 +2157,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O100"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,20 +2191,23 @@
       <c r="K1">
         <v>1</v>
       </c>
-      <c r="M1" s="1">
-        <f>A2*0.4</f>
-        <v>3.6</v>
-      </c>
-      <c r="N1" s="1">
-        <f t="shared" ref="N1:O1" si="0">B2*0.4</f>
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>9</v>
       </c>
@@ -926,19 +2236,26 @@
         <v>2</v>
       </c>
       <c r="M2" s="1">
-        <f t="shared" ref="M2:M65" si="1">A3*0.4</f>
+        <f>A2*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N2" s="1">
-        <f t="shared" ref="N2:N65" si="2">B3*0.4</f>
+        <f>B2*0.4</f>
         <v>4</v>
       </c>
       <c r="O2" s="1">
-        <f t="shared" ref="O2:O65" si="3">C3*0.4</f>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <f>C2*0.4</f>
+        <v>4</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R2">
+        <f t="array" ref="R2:R3">FREQUENCY(M2:M101,Q2:Q3)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>9</v>
       </c>
@@ -967,19 +2284,25 @@
         <v>3</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" si="1"/>
+        <f>A3*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" si="2"/>
+        <f>B3*0.4</f>
         <v>4</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <f>C3*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>9</v>
       </c>
@@ -997,30 +2320,30 @@
         <v>9</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:H4" si="4">MODE(B2:B101)</f>
+        <f t="shared" ref="G4:H4" si="0">MODE(B2:B101)</f>
         <v>10</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="K4">
         <v>4</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="1"/>
+        <f>A4*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="2"/>
+        <f>B4*0.4</f>
         <v>4</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <f>C4*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1034,19 +2357,25 @@
         <v>5</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="1"/>
+        <f>A5*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="2"/>
+        <f>B5*0.4</f>
         <v>4</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <f>C5*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1069,19 +2398,26 @@
         <v>6</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="1"/>
+        <f>A6*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="2"/>
+        <f>B6*0.4</f>
         <v>4</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <f>C6*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <f t="array" ref="R6:R7">FREQUENCY(N2:N101,Q6:Q7)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1099,30 +2435,36 @@
         <v>3.6320000000000001</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:H7" si="5">AVERAGE(B2:B101)*0.4</f>
+        <f t="shared" ref="G7:H7" si="1">AVERAGE(B2:B101)*0.4</f>
         <v>4.0200000000000005</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>4.4400000000000004</v>
       </c>
       <c r="K7">
         <v>7</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="1"/>
+        <f>A7*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="2"/>
+        <f>B7*0.4</f>
         <v>4</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <f>C7*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1140,30 +2482,30 @@
         <v>3.6</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:H8" si="6">MEDIAN(B2:B101)*0.4</f>
+        <f t="shared" ref="G8:H8" si="2">MEDIAN(B2:B101)*0.4</f>
         <v>4</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="K8">
         <v>8</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="1"/>
+        <f>A8*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="2"/>
+        <f>B8*0.4</f>
         <v>4</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <f>C8*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1181,30 +2523,36 @@
         <v>3.6</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:H9" si="7">MODE(B2:B101)*0.4</f>
+        <f t="shared" ref="G9:H9" si="3">MODE(B2:B101)*0.4</f>
         <v>4</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="K9">
         <v>9</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="1"/>
+        <f>A9*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="2"/>
+        <f>B9*0.4</f>
         <v>4</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <f>C9*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1218,19 +2566,26 @@
         <v>10</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="1"/>
+        <f>A10*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="2"/>
+        <f>B10*0.4</f>
         <v>4</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <f>C10*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <f t="array" ref="R10:R12">FREQUENCY(O2:O101,Q10:Q12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1244,19 +2599,25 @@
         <v>11</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="1"/>
+        <f>A11*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="2"/>
+        <f>B11*0.4</f>
         <v>4</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <f>C11*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R11">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1270,19 +2631,25 @@
         <v>12</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="1"/>
+        <f>A12*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="2"/>
+        <f>B12*0.4</f>
         <v>4</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <f>C12*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1296,19 +2663,19 @@
         <v>13</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="1"/>
+        <f>A13*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="2"/>
+        <f>B13*0.4</f>
         <v>4</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <f>C13*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1322,19 +2689,19 @@
         <v>14</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="1"/>
+        <f>A14*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="2"/>
+        <f>B14*0.4</f>
         <v>4</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <f>C14*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1348,19 +2715,19 @@
         <v>15</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="1"/>
+        <f>A15*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="2"/>
+        <f>B15*0.4</f>
         <v>4</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <f>C15*0.4</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1374,15 +2741,15 @@
         <v>16</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="1"/>
+        <f>A16*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="2"/>
+        <f>B16*0.4</f>
         <v>4</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="3"/>
+        <f>C16*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1400,15 +2767,15 @@
         <v>17</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="1"/>
+        <f>A17*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="2"/>
+        <f>B17*0.4</f>
         <v>4</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="3"/>
+        <f>C17*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1426,15 +2793,15 @@
         <v>18</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="1"/>
+        <f>A18*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="2"/>
+        <f>B18*0.4</f>
         <v>4</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="3"/>
+        <f>C18*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1452,15 +2819,15 @@
         <v>19</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="1"/>
+        <f>A19*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="2"/>
+        <f>B19*0.4</f>
         <v>4</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="3"/>
+        <f>C19*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1478,15 +2845,15 @@
         <v>20</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="1"/>
+        <f>A20*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="2"/>
+        <f>B20*0.4</f>
         <v>4</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="3"/>
+        <f>C20*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1504,15 +2871,15 @@
         <v>21</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="1"/>
+        <f>A21*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="2"/>
+        <f>B21*0.4</f>
         <v>4</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="3"/>
+        <f>C21*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1530,15 +2897,15 @@
         <v>22</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="1"/>
+        <f>A22*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="2"/>
+        <f>B22*0.4</f>
         <v>4</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="3"/>
+        <f>C22*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1556,15 +2923,15 @@
         <v>23</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="1"/>
+        <f>A23*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="2"/>
+        <f>B23*0.4</f>
         <v>4</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="3"/>
+        <f>C23*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1582,15 +2949,15 @@
         <v>24</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="1"/>
+        <f>A24*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="2"/>
+        <f>B24*0.4</f>
         <v>4</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="3"/>
+        <f>C24*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1608,15 +2975,15 @@
         <v>25</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="1"/>
+        <f>A25*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="2"/>
+        <f>B25*0.4</f>
         <v>4</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="3"/>
+        <f>C25*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1634,15 +3001,15 @@
         <v>26</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="1"/>
+        <f>A26*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <f>B26*0.4</f>
+        <v>4</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="3"/>
+        <f>C26*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1660,15 +3027,15 @@
         <v>27</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="1"/>
+        <f>A27*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>B27*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="3"/>
+        <f>C27*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1686,15 +3053,15 @@
         <v>28</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="1"/>
+        <f>A28*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="2"/>
+        <f>B28*0.4</f>
         <v>4</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="3"/>
+        <f>C28*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1712,16 +3079,16 @@
         <v>29</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="1"/>
+        <f>A29*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="2"/>
+        <f>B29*0.4</f>
         <v>4</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="3"/>
-        <v>8.8000000000000007</v>
+        <f>C29*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1738,16 +3105,16 @@
         <v>30</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="1"/>
+        <f>A30*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <f>B30*0.4</f>
+        <v>4</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
+        <f>C30*0.4</f>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1764,15 +3131,15 @@
         <v>31</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="1"/>
+        <f>A31*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>B31*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="3"/>
+        <f>C31*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1790,15 +3157,15 @@
         <v>32</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="1"/>
+        <f>A32*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="2"/>
+        <f>B32*0.4</f>
         <v>4</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="3"/>
+        <f>C32*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1816,15 +3183,15 @@
         <v>33</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="1"/>
+        <f>A33*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="2"/>
+        <f>B33*0.4</f>
         <v>4</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="3"/>
+        <f>C33*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1842,15 +3209,15 @@
         <v>34</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="1"/>
+        <f>A34*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="2"/>
+        <f>B34*0.4</f>
         <v>4</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="3"/>
+        <f>C34*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1868,15 +3235,15 @@
         <v>35</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="1"/>
+        <f>A35*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="2"/>
+        <f>B35*0.4</f>
         <v>4</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="3"/>
+        <f>C35*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1894,15 +3261,15 @@
         <v>36</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="1"/>
+        <f>A36*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N36" s="1">
-        <f t="shared" si="2"/>
+        <f>B36*0.4</f>
         <v>4</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="3"/>
+        <f>C36*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1920,15 +3287,15 @@
         <v>37</v>
       </c>
       <c r="M37" s="1">
-        <f t="shared" si="1"/>
+        <f>A37*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N37" s="1">
-        <f t="shared" si="2"/>
+        <f>B37*0.4</f>
         <v>4</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" si="3"/>
+        <f>C37*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1946,15 +3313,15 @@
         <v>38</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="1"/>
+        <f>A38*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N38" s="1">
-        <f t="shared" si="2"/>
+        <f>B38*0.4</f>
         <v>4</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="3"/>
+        <f>C38*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1972,15 +3339,15 @@
         <v>39</v>
       </c>
       <c r="M39" s="1">
-        <f t="shared" si="1"/>
+        <f>A39*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N39" s="1">
-        <f t="shared" si="2"/>
+        <f>B39*0.4</f>
         <v>4</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="3"/>
+        <f>C39*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1998,15 +3365,15 @@
         <v>40</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="1"/>
+        <f>A40*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" si="2"/>
+        <f>B40*0.4</f>
         <v>4</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="3"/>
+        <f>C40*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2024,15 +3391,15 @@
         <v>41</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="1"/>
+        <f>A41*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" si="2"/>
+        <f>B41*0.4</f>
         <v>4</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="3"/>
+        <f>C41*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2050,15 +3417,15 @@
         <v>42</v>
       </c>
       <c r="M42" s="1">
-        <f t="shared" si="1"/>
+        <f>A42*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N42" s="1">
-        <f t="shared" si="2"/>
+        <f>B42*0.4</f>
         <v>4</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="3"/>
+        <f>C42*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2076,15 +3443,15 @@
         <v>43</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="1"/>
+        <f>A43*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N43" s="1">
-        <f t="shared" si="2"/>
+        <f>B43*0.4</f>
         <v>4</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="3"/>
+        <f>C43*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2102,15 +3469,15 @@
         <v>44</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="1"/>
+        <f>A44*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" si="2"/>
+        <f>B44*0.4</f>
         <v>4</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="3"/>
+        <f>C44*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2128,15 +3495,15 @@
         <v>45</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="1"/>
+        <f>A45*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N45" s="1">
-        <f t="shared" si="2"/>
+        <f>B45*0.4</f>
         <v>4</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="3"/>
+        <f>C45*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2154,15 +3521,15 @@
         <v>46</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="1"/>
+        <f>A46*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" si="2"/>
+        <f>B46*0.4</f>
         <v>4</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="3"/>
+        <f>C46*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2180,15 +3547,15 @@
         <v>47</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="1"/>
+        <f>A47*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="2"/>
+        <f>B47*0.4</f>
         <v>4</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="3"/>
+        <f>C47*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2206,15 +3573,15 @@
         <v>48</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="1"/>
+        <f>A48*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N48" s="1">
-        <f t="shared" si="2"/>
+        <f>B48*0.4</f>
         <v>4</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="3"/>
+        <f>C48*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2232,15 +3599,15 @@
         <v>49</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="1"/>
+        <f>A49*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" si="2"/>
+        <f>B49*0.4</f>
         <v>4</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="3"/>
+        <f>C49*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2258,15 +3625,15 @@
         <v>50</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="1"/>
+        <f>A50*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="2"/>
+        <f>B50*0.4</f>
         <v>4</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="3"/>
+        <f>C50*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2284,15 +3651,15 @@
         <v>51</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="1"/>
+        <f>A51*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N51" s="1">
-        <f t="shared" si="2"/>
+        <f>B51*0.4</f>
         <v>4</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="3"/>
+        <f>C51*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2310,15 +3677,15 @@
         <v>52</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" si="1"/>
+        <f>A52*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N52" s="1">
-        <f t="shared" si="2"/>
+        <f>B52*0.4</f>
         <v>4</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="3"/>
+        <f>C52*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2336,15 +3703,15 @@
         <v>53</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" si="1"/>
+        <f>A53*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" si="2"/>
+        <f>B53*0.4</f>
         <v>4</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="3"/>
+        <f>C53*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2362,15 +3729,15 @@
         <v>54</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" si="1"/>
+        <f>A54*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N54" s="1">
-        <f t="shared" si="2"/>
+        <f>B54*0.4</f>
         <v>4</v>
       </c>
       <c r="O54" s="1">
-        <f t="shared" si="3"/>
+        <f>C54*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2388,15 +3755,15 @@
         <v>55</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="1"/>
+        <f>A55*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="2"/>
+        <f>B55*0.4</f>
         <v>4</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="3"/>
+        <f>C55*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2414,15 +3781,15 @@
         <v>56</v>
       </c>
       <c r="M56" s="1">
-        <f t="shared" si="1"/>
+        <f>A56*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N56" s="1">
-        <f t="shared" si="2"/>
+        <f>B56*0.4</f>
         <v>4</v>
       </c>
       <c r="O56" s="1">
-        <f t="shared" si="3"/>
+        <f>C56*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2440,15 +3807,15 @@
         <v>57</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="1"/>
+        <f>A57*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N57" s="1">
-        <f t="shared" si="2"/>
+        <f>B57*0.4</f>
         <v>4</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="3"/>
+        <f>C57*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2466,15 +3833,15 @@
         <v>58</v>
       </c>
       <c r="M58" s="1">
-        <f t="shared" si="1"/>
+        <f>A58*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N58" s="1">
-        <f t="shared" si="2"/>
+        <f>B58*0.4</f>
         <v>4</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="3"/>
+        <f>C58*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2492,15 +3859,15 @@
         <v>59</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" si="1"/>
+        <f>A59*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N59" s="1">
-        <f t="shared" si="2"/>
+        <f>B59*0.4</f>
         <v>4</v>
       </c>
       <c r="O59" s="1">
-        <f t="shared" si="3"/>
+        <f>C59*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2518,15 +3885,15 @@
         <v>60</v>
       </c>
       <c r="M60" s="1">
-        <f t="shared" si="1"/>
+        <f>A60*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N60" s="1">
-        <f t="shared" si="2"/>
+        <f>B60*0.4</f>
         <v>4</v>
       </c>
       <c r="O60" s="1">
-        <f t="shared" si="3"/>
+        <f>C60*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2544,15 +3911,15 @@
         <v>61</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="1"/>
+        <f>A61*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N61" s="1">
-        <f t="shared" si="2"/>
+        <f>B61*0.4</f>
         <v>4</v>
       </c>
       <c r="O61" s="1">
-        <f t="shared" si="3"/>
+        <f>C61*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2570,15 +3937,15 @@
         <v>62</v>
       </c>
       <c r="M62" s="1">
-        <f t="shared" si="1"/>
+        <f>A62*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N62" s="1">
-        <f t="shared" si="2"/>
+        <f>B62*0.4</f>
         <v>4</v>
       </c>
       <c r="O62" s="1">
-        <f t="shared" si="3"/>
+        <f>C62*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2596,15 +3963,15 @@
         <v>63</v>
       </c>
       <c r="M63" s="1">
-        <f t="shared" si="1"/>
+        <f>A63*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N63" s="1">
-        <f t="shared" si="2"/>
+        <f>B63*0.4</f>
         <v>4</v>
       </c>
       <c r="O63" s="1">
-        <f t="shared" si="3"/>
+        <f>C63*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2622,15 +3989,15 @@
         <v>64</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" si="1"/>
+        <f>A64*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N64" s="1">
-        <f t="shared" si="2"/>
+        <f>B64*0.4</f>
         <v>4</v>
       </c>
       <c r="O64" s="1">
-        <f t="shared" si="3"/>
+        <f>C64*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2648,15 +4015,15 @@
         <v>65</v>
       </c>
       <c r="M65" s="1">
-        <f t="shared" si="1"/>
+        <f>A65*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N65" s="1">
-        <f t="shared" si="2"/>
+        <f>B65*0.4</f>
         <v>4</v>
       </c>
       <c r="O65" s="1">
-        <f t="shared" si="3"/>
+        <f>C65*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2674,15 +4041,15 @@
         <v>66</v>
       </c>
       <c r="M66" s="1">
-        <f t="shared" ref="M66:M100" si="8">A67*0.4</f>
+        <f>A66*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N66" s="1">
-        <f t="shared" ref="N66:N100" si="9">B67*0.4</f>
+        <f>B66*0.4</f>
         <v>4</v>
       </c>
       <c r="O66" s="1">
-        <f t="shared" ref="O66:O100" si="10">C67*0.4</f>
+        <f>C66*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2700,15 +4067,15 @@
         <v>67</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" si="8"/>
+        <f>A67*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N67" s="1">
-        <f t="shared" si="9"/>
-        <v>4.4000000000000004</v>
+        <f>B67*0.4</f>
+        <v>4</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="10"/>
+        <f>C67*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2726,15 +4093,15 @@
         <v>68</v>
       </c>
       <c r="M68" s="1">
-        <f t="shared" si="8"/>
+        <f>A68*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N68" s="1">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f>B68*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O68" s="1">
-        <f t="shared" si="10"/>
+        <f>C68*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2752,15 +4119,15 @@
         <v>69</v>
       </c>
       <c r="M69" s="1">
-        <f t="shared" si="8"/>
+        <f>A69*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N69" s="1">
-        <f t="shared" si="9"/>
+        <f>B69*0.4</f>
         <v>4</v>
       </c>
       <c r="O69" s="1">
-        <f t="shared" si="10"/>
+        <f>C69*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2778,15 +4145,15 @@
         <v>70</v>
       </c>
       <c r="M70" s="1">
-        <f t="shared" si="8"/>
+        <f>A70*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N70" s="1">
-        <f t="shared" si="9"/>
+        <f>B70*0.4</f>
         <v>4</v>
       </c>
       <c r="O70" s="1">
-        <f t="shared" si="10"/>
+        <f>C70*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2804,15 +4171,15 @@
         <v>71</v>
       </c>
       <c r="M71" s="1">
-        <f t="shared" si="8"/>
+        <f>A71*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" si="9"/>
-        <v>4.4000000000000004</v>
+        <f>B71*0.4</f>
+        <v>4</v>
       </c>
       <c r="O71" s="1">
-        <f t="shared" si="10"/>
+        <f>C71*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2830,15 +4197,15 @@
         <v>72</v>
       </c>
       <c r="M72" s="1">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f>A72*0.4</f>
+        <v>3.6</v>
       </c>
       <c r="N72" s="1">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f>B72*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O72" s="1">
-        <f t="shared" si="10"/>
+        <f>C72*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2856,15 +4223,15 @@
         <v>73</v>
       </c>
       <c r="M73" s="1">
-        <f t="shared" si="8"/>
+        <f>A73*0.4</f>
         <v>4</v>
       </c>
       <c r="N73" s="1">
-        <f t="shared" si="9"/>
+        <f>B73*0.4</f>
         <v>4</v>
       </c>
       <c r="O73" s="1">
-        <f t="shared" si="10"/>
+        <f>C73*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2882,15 +4249,15 @@
         <v>74</v>
       </c>
       <c r="M74" s="1">
-        <f t="shared" si="8"/>
+        <f>A74*0.4</f>
         <v>4</v>
       </c>
       <c r="N74" s="1">
-        <f t="shared" si="9"/>
+        <f>B74*0.4</f>
         <v>4</v>
       </c>
       <c r="O74" s="1">
-        <f t="shared" si="10"/>
+        <f>C74*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2908,15 +4275,15 @@
         <v>75</v>
       </c>
       <c r="M75" s="1">
-        <f t="shared" si="8"/>
+        <f>A75*0.4</f>
         <v>4</v>
       </c>
       <c r="N75" s="1">
-        <f t="shared" si="9"/>
+        <f>B75*0.4</f>
         <v>4</v>
       </c>
       <c r="O75" s="1">
-        <f t="shared" si="10"/>
+        <f>C75*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2934,15 +4301,15 @@
         <v>76</v>
       </c>
       <c r="M76" s="1">
-        <f t="shared" si="8"/>
+        <f>A76*0.4</f>
         <v>4</v>
       </c>
       <c r="N76" s="1">
-        <f t="shared" si="9"/>
+        <f>B76*0.4</f>
         <v>4</v>
       </c>
       <c r="O76" s="1">
-        <f t="shared" si="10"/>
+        <f>C76*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2960,15 +4327,15 @@
         <v>77</v>
       </c>
       <c r="M77" s="1">
-        <f t="shared" si="8"/>
+        <f>A77*0.4</f>
         <v>4</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="9"/>
+        <f>B77*0.4</f>
         <v>4</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="10"/>
+        <f>C77*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2986,15 +4353,15 @@
         <v>78</v>
       </c>
       <c r="M78" s="1">
-        <f t="shared" si="8"/>
+        <f>A78*0.4</f>
         <v>4</v>
       </c>
       <c r="N78" s="1">
-        <f t="shared" si="9"/>
+        <f>B78*0.4</f>
         <v>4</v>
       </c>
       <c r="O78" s="1">
-        <f t="shared" si="10"/>
+        <f>C78*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3012,15 +4379,15 @@
         <v>79</v>
       </c>
       <c r="M79" s="1">
-        <f t="shared" si="8"/>
+        <f>A79*0.4</f>
         <v>4</v>
       </c>
       <c r="N79" s="1">
-        <f t="shared" si="9"/>
+        <f>B79*0.4</f>
         <v>4</v>
       </c>
       <c r="O79" s="1">
-        <f t="shared" si="10"/>
+        <f>C79*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3038,15 +4405,15 @@
         <v>80</v>
       </c>
       <c r="M80" s="1">
-        <f t="shared" si="8"/>
-        <v>3.6</v>
+        <f>A80*0.4</f>
+        <v>4</v>
       </c>
       <c r="N80" s="1">
-        <f t="shared" si="9"/>
+        <f>B80*0.4</f>
         <v>4</v>
       </c>
       <c r="O80" s="1">
-        <f t="shared" si="10"/>
+        <f>C80*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3064,15 +4431,15 @@
         <v>81</v>
       </c>
       <c r="M81" s="1">
-        <f t="shared" si="8"/>
+        <f>A81*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N81" s="1">
-        <f t="shared" si="9"/>
+        <f>B81*0.4</f>
         <v>4</v>
       </c>
       <c r="O81" s="1">
-        <f t="shared" si="10"/>
+        <f>C81*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3090,15 +4457,15 @@
         <v>82</v>
       </c>
       <c r="M82" s="1">
-        <f t="shared" si="8"/>
+        <f>A82*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N82" s="1">
-        <f t="shared" si="9"/>
+        <f>B82*0.4</f>
         <v>4</v>
       </c>
       <c r="O82" s="1">
-        <f t="shared" si="10"/>
+        <f>C82*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3116,15 +4483,15 @@
         <v>83</v>
       </c>
       <c r="M83" s="1">
-        <f t="shared" si="8"/>
+        <f>A83*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N83" s="1">
-        <f t="shared" si="9"/>
-        <v>4.4000000000000004</v>
+        <f>B83*0.4</f>
+        <v>4</v>
       </c>
       <c r="O83" s="1">
-        <f t="shared" si="10"/>
+        <f>C83*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3142,15 +4509,15 @@
         <v>84</v>
       </c>
       <c r="M84" s="1">
-        <f t="shared" si="8"/>
+        <f>A84*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N84" s="1">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f>B84*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O84" s="1">
-        <f t="shared" si="10"/>
+        <f>C84*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3168,15 +4535,15 @@
         <v>85</v>
       </c>
       <c r="M85" s="1">
-        <f t="shared" si="8"/>
+        <f>A85*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N85" s="1">
-        <f t="shared" si="9"/>
+        <f>B85*0.4</f>
         <v>4</v>
       </c>
       <c r="O85" s="1">
-        <f t="shared" si="10"/>
+        <f>C85*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3194,15 +4561,15 @@
         <v>86</v>
       </c>
       <c r="M86" s="1">
-        <f t="shared" si="8"/>
+        <f>A86*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N86" s="1">
-        <f t="shared" si="9"/>
+        <f>B86*0.4</f>
         <v>4</v>
       </c>
       <c r="O86" s="1">
-        <f t="shared" si="10"/>
+        <f>C86*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3220,15 +4587,15 @@
         <v>87</v>
       </c>
       <c r="M87" s="1">
-        <f t="shared" si="8"/>
+        <f>A87*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N87" s="1">
-        <f t="shared" si="9"/>
+        <f>B87*0.4</f>
         <v>4</v>
       </c>
       <c r="O87" s="1">
-        <f t="shared" si="10"/>
+        <f>C87*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3246,15 +4613,15 @@
         <v>88</v>
       </c>
       <c r="M88" s="1">
-        <f t="shared" si="8"/>
+        <f>A88*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N88" s="1">
-        <f t="shared" si="9"/>
+        <f>B88*0.4</f>
         <v>4</v>
       </c>
       <c r="O88" s="1">
-        <f t="shared" si="10"/>
+        <f>C88*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3272,15 +4639,15 @@
         <v>89</v>
       </c>
       <c r="M89" s="1">
-        <f t="shared" si="8"/>
+        <f>A89*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N89" s="1">
-        <f t="shared" si="9"/>
+        <f>B89*0.4</f>
         <v>4</v>
       </c>
       <c r="O89" s="1">
-        <f t="shared" si="10"/>
+        <f>C89*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3298,15 +4665,15 @@
         <v>90</v>
       </c>
       <c r="M90" s="1">
-        <f t="shared" si="8"/>
+        <f>A90*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N90" s="1">
-        <f t="shared" si="9"/>
+        <f>B90*0.4</f>
         <v>4</v>
       </c>
       <c r="O90" s="1">
-        <f t="shared" si="10"/>
+        <f>C90*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3324,15 +4691,15 @@
         <v>91</v>
       </c>
       <c r="M91" s="1">
-        <f t="shared" si="8"/>
+        <f>A91*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N91" s="1">
-        <f t="shared" si="9"/>
+        <f>B91*0.4</f>
         <v>4</v>
       </c>
       <c r="O91" s="1">
-        <f t="shared" si="10"/>
+        <f>C91*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3350,15 +4717,15 @@
         <v>92</v>
       </c>
       <c r="M92" s="1">
-        <f t="shared" si="8"/>
+        <f>A92*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N92" s="1">
-        <f t="shared" si="9"/>
+        <f>B92*0.4</f>
         <v>4</v>
       </c>
       <c r="O92" s="1">
-        <f t="shared" si="10"/>
+        <f>C92*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3376,15 +4743,15 @@
         <v>93</v>
       </c>
       <c r="M93" s="1">
-        <f t="shared" si="8"/>
+        <f>A93*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N93" s="1">
-        <f t="shared" si="9"/>
+        <f>B93*0.4</f>
         <v>4</v>
       </c>
       <c r="O93" s="1">
-        <f t="shared" si="10"/>
+        <f>C93*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3402,15 +4769,15 @@
         <v>94</v>
       </c>
       <c r="M94" s="1">
-        <f t="shared" si="8"/>
+        <f>A94*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N94" s="1">
-        <f t="shared" si="9"/>
+        <f>B94*0.4</f>
         <v>4</v>
       </c>
       <c r="O94" s="1">
-        <f t="shared" si="10"/>
+        <f>C94*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3428,15 +4795,15 @@
         <v>95</v>
       </c>
       <c r="M95" s="1">
-        <f t="shared" si="8"/>
+        <f>A95*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N95" s="1">
-        <f t="shared" si="9"/>
+        <f>B95*0.4</f>
         <v>4</v>
       </c>
       <c r="O95" s="1">
-        <f t="shared" si="10"/>
+        <f>C95*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3454,15 +4821,15 @@
         <v>96</v>
       </c>
       <c r="M96" s="1">
-        <f t="shared" si="8"/>
+        <f>A96*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N96" s="1">
-        <f t="shared" si="9"/>
+        <f>B96*0.4</f>
         <v>4</v>
       </c>
       <c r="O96" s="1">
-        <f t="shared" si="10"/>
+        <f>C96*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3480,15 +4847,15 @@
         <v>97</v>
       </c>
       <c r="M97" s="1">
-        <f t="shared" si="8"/>
+        <f>A97*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N97" s="1">
-        <f t="shared" si="9"/>
+        <f>B97*0.4</f>
         <v>4</v>
       </c>
       <c r="O97" s="1">
-        <f t="shared" si="10"/>
+        <f>C97*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3506,15 +4873,15 @@
         <v>98</v>
       </c>
       <c r="M98" s="1">
-        <f t="shared" si="8"/>
+        <f>A98*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N98" s="1">
-        <f t="shared" si="9"/>
+        <f>B98*0.4</f>
         <v>4</v>
       </c>
       <c r="O98" s="1">
-        <f t="shared" si="10"/>
+        <f>C98*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3532,15 +4899,15 @@
         <v>99</v>
       </c>
       <c r="M99" s="1">
-        <f t="shared" si="8"/>
+        <f>A99*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N99" s="1">
-        <f t="shared" si="9"/>
+        <f>B99*0.4</f>
         <v>4</v>
       </c>
       <c r="O99" s="1">
-        <f t="shared" si="10"/>
+        <f>C99*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3558,15 +4925,15 @@
         <v>100</v>
       </c>
       <c r="M100" s="1">
-        <f t="shared" si="8"/>
+        <f>A100*0.4</f>
         <v>3.6</v>
       </c>
       <c r="N100" s="1">
-        <f t="shared" si="9"/>
+        <f>B100*0.4</f>
         <v>4</v>
       </c>
       <c r="O100" s="1">
-        <f t="shared" si="10"/>
+        <f>C100*0.4</f>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3579,6 +4946,18 @@
       </c>
       <c r="C101">
         <v>11</v>
+      </c>
+      <c r="M101" s="1">
+        <f>A101*0.4</f>
+        <v>3.6</v>
+      </c>
+      <c r="N101" s="1">
+        <f>B101*0.4</f>
+        <v>4</v>
+      </c>
+      <c r="O101" s="1">
+        <f>C101*0.4</f>
+        <v>4.4000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>